<commit_message>
views to opt. constraints implemented, but thus far only for mean-values
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Nextcloud\Aktia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Documents\Git\entropy-poolin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE7D485-7C85-4BE3-9B67-47B5D3FE9FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9BE56A-74FD-42C5-850A-80675DDF9EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17016" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Asset 3</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>European Equities</t>
-  </si>
-  <si>
-    <t>&lt;</t>
   </si>
   <si>
     <t>EM Equities</t>
@@ -478,7 +475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,31 +490,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -527,8 +524,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E2" s="1">
         <v>5.3999999999999999E-2</v>
@@ -538,7 +535,7 @@
       </c>
       <c r="I2" t="str">
         <f>IF(A2="mean","Mean('"&amp;B2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2+1&amp;" Mean('"&amp;F2&amp;"')"),) &amp; IF(A2="corr","Corr('"&amp;B2&amp;"', '"&amp;C2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2+1&amp;" Corr('"&amp;F2&amp;"', '"&amp;G2&amp;"')"),)</f>
-        <v>Mean('European Equities') &lt; 0,054</v>
+        <v>Mean('European Equities') = 0,054</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -549,20 +546,20 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
         <v>-5.3999999999999999E-2</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="7">
         <v>1</v>
       </c>
       <c r="I3" t="str">
         <f>IF(A3="mean","Mean('"&amp;B3&amp;"') "&amp;D3&amp;" "&amp;IF(ISBLANK(F3),E3,E3+1&amp;" Mean('"&amp;F3&amp;"')"),) &amp; IF(A3="corr","Corr('"&amp;B3&amp;"', '"&amp;C3&amp;"') "&amp;D3&amp;" "&amp;IF(ISBLANK(F3),E3,E3+1&amp;" Corr('"&amp;F3&amp;"', '"&amp;G3&amp;"')"),)</f>
-        <v>Mean('European Equities') &lt; 0,946 Mean('EM Equities')</v>
+        <v>Mean('European Equities') = 0,946 Mean('EM Equities')</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -570,19 +567,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
         <v>-5.3999999999999999E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -600,13 +597,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
         <v>0.4</v>
@@ -632,12 +629,12 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Covariance constraints implemented, but not yet tested for bugs
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Documents\Git\entropy-poolin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9BE56A-74FD-42C5-850A-80675DDF9EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495700D7-0717-416D-BCA4-DEDC47B58774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17016" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12300" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Asset 3</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Weight (0-100%)</t>
+  </si>
+  <si>
+    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1">
         <v>-5.3999999999999999E-2</v>
@@ -559,7 +562,7 @@
       </c>
       <c r="I3" t="str">
         <f>IF(A3="mean","Mean('"&amp;B3&amp;"') "&amp;D3&amp;" "&amp;IF(ISBLANK(F3),E3,E3+1&amp;" Mean('"&amp;F3&amp;"')"),) &amp; IF(A3="corr","Corr('"&amp;B3&amp;"', '"&amp;C3&amp;"') "&amp;D3&amp;" "&amp;IF(ISBLANK(F3),E3,E3+1&amp;" Corr('"&amp;F3&amp;"', '"&amp;G3&amp;"')"),)</f>
-        <v>Mean('European Equities') = 0,946 Mean('EM Equities')</v>
+        <v>Mean('European Equities') &lt; 0,946 Mean('EM Equities')</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
relative views redefined, they make better sense now; code cleaned
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Documents\Git\entropy-poolin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495700D7-0717-416D-BCA4-DEDC47B58774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F855E51-1ADC-40D5-82D8-507A71E0289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12300" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="22656" windowHeight="12096" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Asset 3</t>
   </si>
@@ -82,13 +82,16 @@
     <t>Preview</t>
   </si>
   <si>
-    <t>Parametrin yksikkö on %, paitsi yksipuoleisessa Cov-tapauksessa</t>
-  </si>
-  <si>
     <t>Weight (0-100%)</t>
   </si>
   <si>
     <t>&lt;</t>
+  </si>
+  <si>
+    <t>Parametrin yksikkö on % tai kovarianssin yksikkö (%^2)</t>
+  </si>
+  <si>
+    <t>DM Equities</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>14</v>
@@ -537,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="str">
-        <f>IF(A2="mean","Mean('"&amp;B2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2+1&amp;" Mean('"&amp;F2&amp;"')"),) &amp; IF(A2="corr","Corr('"&amp;B2&amp;"', '"&amp;C2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2+1&amp;" Corr('"&amp;F2&amp;"', '"&amp;G2&amp;"')"),)</f>
+        <f t="shared" ref="I2:I5" si="0">IF(A2="mean","Mean('"&amp;B2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2&amp;" + Mean('"&amp;F2&amp;"')"),) &amp; IF(A2="cov","Cov('"&amp;B2&amp;"', '"&amp;C2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2&amp;" + Cov('"&amp;F2&amp;"', '"&amp;G2&amp;"')"),)</f>
         <v>Mean('European Equities') = 0,054</v>
       </c>
     </row>
@@ -549,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
         <v>-5.3999999999999999E-2</v>
@@ -561,8 +564,8 @@
         <v>1</v>
       </c>
       <c r="I3" t="str">
-        <f>IF(A3="mean","Mean('"&amp;B3&amp;"') "&amp;D3&amp;" "&amp;IF(ISBLANK(F3),E3,E3+1&amp;" Mean('"&amp;F3&amp;"')"),) &amp; IF(A3="corr","Corr('"&amp;B3&amp;"', '"&amp;C3&amp;"') "&amp;D3&amp;" "&amp;IF(ISBLANK(F3),E3,E3+1&amp;" Corr('"&amp;F3&amp;"', '"&amp;G3&amp;"')"),)</f>
-        <v>Mean('European Equities') &lt; 0,946 Mean('EM Equities')</v>
+        <f t="shared" si="0"/>
+        <v>Mean('European Equities') &lt; -0,054 + Mean('EM Equities')</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -582,7 +585,7 @@
         <v>-5.3999999999999999E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -591,8 +594,8 @@
         <v>0.9</v>
       </c>
       <c r="I4" t="str">
-        <f>IF(A4="mean","Mean('"&amp;B4&amp;"') "&amp;D4&amp;" "&amp;IF(ISBLANK(F4),E4,E4+1&amp;" Mean('"&amp;F4&amp;"')"),) &amp; IF(A4="cov","Cov('"&amp;B4&amp;"', '"&amp;C4&amp;"') "&amp;D4&amp;" "&amp;IF(ISBLANK(F4),E4,E4+1&amp;" Cov('"&amp;F4&amp;"', '"&amp;G4&amp;"')"),)</f>
-        <v>Cov('EM Equities', 'European Equities') = 0,946 Cov('EM Equities', 'European Equities')</v>
+        <f>IF(A4="mean","Mean('"&amp;B4&amp;"') "&amp;D4&amp;" "&amp;IF(ISBLANK(F4),E4,E4&amp;" + Mean('"&amp;F4&amp;"')"),) &amp; IF(A4="cov","Cov('"&amp;B4&amp;"', '"&amp;C4&amp;"') "&amp;D4&amp;" "&amp;IF(ISBLANK(F4),E4,E4&amp;" + Cov('"&amp;F4&amp;"', '"&amp;G4&amp;"')"),)</f>
+        <v>Cov('EM Equities', 'European Equities') = -0,054 + Cov('DM Equities', 'European Equities')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -615,7 +618,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" t="str">
-        <f>IF(A5="mean","Mean('"&amp;B5&amp;"') "&amp;D5&amp;" "&amp;IF(ISBLANK(F5),E5,E5+1&amp;" Mean('"&amp;F5&amp;"')"),) &amp; IF(A5="cov","Cov('"&amp;B5&amp;"', '"&amp;C5&amp;"') "&amp;D5&amp;" "&amp;IF(ISBLANK(F5),E5,E5+1&amp;" Cov('"&amp;F5&amp;"', '"&amp;G5&amp;"')"),)</f>
+        <f t="shared" si="0"/>
         <v>Cov('EM Equities', 'European Equities') &gt; 0,4</v>
       </c>
     </row>
@@ -637,7 +640,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Views functionality updated to the client's needs
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Documents\Git\entropy-poolin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F855E51-1ADC-40D5-82D8-507A71E0289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5151BA3-A0D4-4080-B62C-124D5A6CFCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="22656" windowHeight="12096" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="23040" windowHeight="12300" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="views" sheetId="1" r:id="rId1"/>
+    <sheet name="input validation" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="factor">'input validation'!$B$2:$B$37</definedName>
+    <definedName name="factor_2">'input validation'!$B$1:$B$37</definedName>
+    <definedName name="operator">'input validation'!$C$1:$C$5</definedName>
+    <definedName name="type">'input validation'!$A$1:$A$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,16 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
-  <si>
-    <t>Asset 3</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>cov</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>European Equities</t>
   </si>
@@ -52,52 +49,173 @@
     <t>EM Equities</t>
   </si>
   <si>
-    <t>Asset 2 (only cov)</t>
-  </si>
-  <si>
-    <t>Asset 4 (only cov)</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
     <t>&gt;</t>
   </si>
   <si>
-    <t>*Asset 1</t>
-  </si>
-  <si>
-    <t>*eq / ineq</t>
-  </si>
-  <si>
-    <t>*Parameter (% or cov)</t>
-  </si>
-  <si>
-    <t>*View type (mean/cov)</t>
-  </si>
-  <si>
-    <t>Jos samat vas. Ja oik. puolella, niin ottaa vanhasta arvon ja muuttaa sitä</t>
-  </si>
-  <si>
     <t>Preview</t>
   </si>
   <si>
-    <t>Weight (0-100%)</t>
-  </si>
-  <si>
     <t>&lt;</t>
   </si>
   <si>
-    <t>Parametrin yksikkö on % tai kovarianssin yksikkö (%^2)</t>
-  </si>
-  <si>
     <t>DM Equities</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>* Risk factor 1</t>
+  </si>
+  <si>
+    <t>* View on</t>
+  </si>
+  <si>
+    <t>Risk factor 3</t>
+  </si>
+  <si>
+    <t>* Operator</t>
+  </si>
+  <si>
+    <t>Global Equities</t>
+  </si>
+  <si>
+    <t>US Equities</t>
+  </si>
+  <si>
+    <t>EUR Money Markets</t>
+  </si>
+  <si>
+    <t>EUR Government Bonds</t>
+  </si>
+  <si>
+    <t>EUR Covered Bonds</t>
+  </si>
+  <si>
+    <t>EUR Investment Grade Corporate Bonds</t>
+  </si>
+  <si>
+    <t>European High Yield Corporate Bonds</t>
+  </si>
+  <si>
+    <t>EMD Hard Currency</t>
+  </si>
+  <si>
+    <t>Hedge Funds</t>
+  </si>
+  <si>
+    <t>Listed Private Equity</t>
+  </si>
+  <si>
+    <t>1Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>2Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>3Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>5Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>7Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>10Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>15Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>20Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>30Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>50Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>US 10-Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>Germany 10-Year Government Bond Yield</t>
+  </si>
+  <si>
+    <t>iVol US Equities</t>
+  </si>
+  <si>
+    <t>iVol European Equities</t>
+  </si>
+  <si>
+    <t>FED Balance Sheet Total</t>
+  </si>
+  <si>
+    <t>Eurosystem Balance Sheet Total</t>
+  </si>
+  <si>
+    <t>US Core Inflation</t>
+  </si>
+  <si>
+    <t>US Unemployment</t>
+  </si>
+  <si>
+    <t>US Manufacturing PMI</t>
+  </si>
+  <si>
+    <t>US Services PMI</t>
+  </si>
+  <si>
+    <t>Eurozone Core Inflation</t>
+  </si>
+  <si>
+    <t>Eurozone Unemployment</t>
+  </si>
+  <si>
+    <t>Risk factor 2 
+(applicable for corr)</t>
+  </si>
+  <si>
+    <t>Risk factor 4 
+(applicable for corr)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>* Constant 
+(alpha)</t>
+  </si>
+  <si>
+    <t>Multiplier 
+(beta)</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Vol</t>
+  </si>
+  <si>
+    <t>Corr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,32 +261,242 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
     <cellStyle name="Prosenttia" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="21">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC7CE"/>
+      <color rgb="FF9C0006"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -178,6 +506,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E8D6B3D-41D7-44A8-A9B4-14D70EA53777}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:I5" xr:uid="{0E8D6B3D-41D7-44A8-A9B4-14D70EA53777}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{FCA19E57-E117-4192-A175-C5A846A4971B}" name="* View on"/>
+    <tableColumn id="2" xr3:uid="{7E3FD807-66CB-4DA9-9133-3EC201CA09A8}" name="* Risk factor 1"/>
+    <tableColumn id="3" xr3:uid="{2F98A85F-03A4-450D-8AF2-3B362213618B}" name="Risk factor 2 _x000a_(applicable for corr)"/>
+    <tableColumn id="4" xr3:uid="{4A5D765B-9D0B-4E55-9534-B8A4D4FC2C1F}" name="* Operator" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{AC255133-F992-4D98-BA26-B8BD35806503}" name="* Constant _x000a_(alpha)" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{58720F09-B85A-47FB-90E4-1704206B41AB}" name="Multiplier _x000a_(beta)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{71DCC6EE-632C-440A-8DDD-79D249B08D41}" name="Risk factor 3"/>
+    <tableColumn id="8" xr3:uid="{400671E3-F507-48B3-979B-9E6581D2ECF2}" name="Risk factor 4 _x000a_(applicable for corr)"/>
+    <tableColumn id="9" xr3:uid="{D16B2553-BDA4-4084-B6CC-37585AC8BB8F}" name="Preview" dataDxfId="0">
+      <calculatedColumnFormula>IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
+&amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
+&amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,154 +827,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D192AB-C94F-4991-A9BC-7033E27831F6}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>14</v>
+      <c r="H1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I5" si="0">IF(A2="mean","Mean('"&amp;B2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2&amp;" + Mean('"&amp;F2&amp;"')"),) &amp; IF(A2="cov","Cov('"&amp;B2&amp;"', '"&amp;C2&amp;"') "&amp;D2&amp;" "&amp;IF(ISBLANK(F2),E2,E2&amp;" + Cov('"&amp;F2&amp;"', '"&amp;G2&amp;"')"),)</f>
-        <v>Mean('European Equities') = 0,054</v>
+        <f t="shared" ref="I2:I5" si="0">IF(A2="mean","μ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"μ_"&amp;G2&amp;" (p.a.)"),"")
+&amp;IF(A2="vol","σ_"&amp;B2&amp;" (p.a.) "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"σ_"&amp;G2&amp;" (p.a.)"),"")
+&amp;IF(A2="corr","ρ("&amp;B2&amp;", "&amp;C2&amp;") "&amp;D2&amp;" "&amp;IF(E2=0,"",E2&amp;" ")&amp;IF(OR(G2="-",F2=0),"",IF(E2=0,"","+")&amp;" "&amp;IF(F2=1,"",F2)&amp;"ρ("&amp;G2&amp;", "&amp;H2&amp;")"),"")</f>
+        <v xml:space="preserve">μ_European Equities (p.a.) = 0,05 </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-5.3999999999999999E-2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v>Mean('European Equities') &lt; -0,054 + Mean('EM Equities')</v>
+        <v>σ_European Equities (p.a.) &lt; 0,1 + σ_Global Equities (p.a.)</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-5.3999999999999999E-2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
+      <c r="E4" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.9</v>
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
       </c>
       <c r="I4" t="str">
-        <f>IF(A4="mean","Mean('"&amp;B4&amp;"') "&amp;D4&amp;" "&amp;IF(ISBLANK(F4),E4,E4&amp;" + Mean('"&amp;F4&amp;"')"),) &amp; IF(A4="cov","Cov('"&amp;B4&amp;"', '"&amp;C4&amp;"') "&amp;D4&amp;" "&amp;IF(ISBLANK(F4),E4,E4&amp;" + Cov('"&amp;F4&amp;"', '"&amp;G4&amp;"')"),)</f>
-        <v>Cov('EM Equities', 'European Equities') = -0,054 + Cov('DM Equities', 'European Equities')</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ρ(European Equities, Global Equities) = 0,9 </v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.1</v>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>Cov('EM Equities', 'European Equities') &gt; 0,4</v>
+        <v>ρ(EM Equities, European Equities) &gt;  0,5ρ(Global Equities, Global Equities)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
@@ -634,17 +1011,312 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
-      <c r="I9" t="s">
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="expression" dxfId="20" priority="22">
+      <formula>AND($A2="vol",C2&lt;&gt;"-")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="23">
+      <formula>AND($A2="corr",C2="-")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="34">
+      <formula>AND($A2="mean",C2&lt;&gt;"-")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C5">
+    <cfRule type="expression" dxfId="17" priority="32">
+      <formula>AND($A3="Corr",$C3="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>AND($A2="corr",E2&gt;1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>AND($A2="vol",E2&lt;=0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>AND($A2="corr",E2&lt;-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>AND($A2="vol",H2&lt;&gt;"-")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>AND($A2="corr",H2="-")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>AND($A2="mean",H2&lt;&gt;"-")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H5">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>AND($A3="vol",H3&lt;&gt;"-")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>AND($A3="corr",H3="-")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>AND($A3="mean",H3&lt;&gt;"-")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E6">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>AND($A3="corr",E3&gt;1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>AND($A3="vol",E3&lt;=0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>AND($A3="corr",E3&lt;-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{1BD6A80F-057B-42B5-ABFC-45CECF7EF490}">
+      <formula1>type</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{575793F7-C0C6-49FB-A3FE-44818B4359F8}">
+      <formula1>factor</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 G2:H5" xr:uid="{D6AD6B0E-76FB-4811-89E0-4A267DE08065}">
+      <formula1>factor_2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{49E95D0B-EF72-4117-B5C9-1FB8FBB1A873}">
+      <formula1>operator</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEABC6F7-BCA1-46E3-8462-01F3C233635C}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
views modified to meet customer's specifications; lot of cleaning
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapam\Documents\Git\entropy-poolin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5151BA3-A0D4-4080-B62C-124D5A6CFCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865AD180-0C63-4575-B789-71F7A69AC10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="23040" windowHeight="12300" xr2:uid="{947BAB4B-B7D2-4750-A7BC-B652DF564494}"/>
   </bookViews>
@@ -831,7 +831,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
@@ -1077,10 +1077,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{1BD6A80F-057B-42B5-ABFC-45CECF7EF490}">
       <formula1>type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{575793F7-C0C6-49FB-A3FE-44818B4359F8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5 G4" xr:uid="{575793F7-C0C6-49FB-A3FE-44818B4359F8}">
       <formula1>factor</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 G2:H5" xr:uid="{D6AD6B0E-76FB-4811-89E0-4A267DE08065}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 H2:H5 G2:G3 G5" xr:uid="{D6AD6B0E-76FB-4811-89E0-4A267DE08065}">
       <formula1>factor_2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{49E95D0B-EF72-4117-B5C9-1FB8FBB1A873}">

</xml_diff>